<commit_message>
Added Test Cases for Training.
</commit_message>
<xml_diff>
--- a/TestData/VT-CC-Transactions.xlsx
+++ b/TestData/VT-CC-Transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UIPath\VPSAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5EC882-2205-4C32-84A5-D047D1BF5D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA4C291-9D68-4715-B142-F4F4C395B1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="2490" windowWidth="24525" windowHeight="14010" xr2:uid="{38671F56-4198-4E87-B365-8D39954119AF}"/>
+    <workbookView xWindow="37290" yWindow="2685" windowWidth="15360" windowHeight="8670" xr2:uid="{38671F56-4198-4E87-B365-8D39954119AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,10 +260,10 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>02/25/2024 22:16:38</t>
-  </si>
-  <si>
     <t>02/25/2024 22:17:46</t>
+  </si>
+  <si>
+    <t>04/25/2024 19:57:28</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
         <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>31</v>
@@ -949,7 +949,7 @@
         <v>73</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>

</xml_diff>